<commit_message>
Update Reader PCB Parts List.xlsx
Changed ADMIT and REJECT LEDs to be backlit panel buttons (per team meeting 8/16/19)
</commit_message>
<xml_diff>
--- a/Hardware/Reader PCB Parts List.xlsx
+++ b/Hardware/Reader PCB Parts List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bobg5\Documents\Bob\Hobby\MN ACL\Reader_PCB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C985AE94-6E1F-48E1-86A6-543FAACA506B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA798988-A76C-4921-82EC-2DEA438D06E5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{767E0BC8-B2C0-4E54-85D5-C5F8ECA18261}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{767E0BC8-B2C0-4E54-85D5-C5F8ECA18261}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="68">
   <si>
     <t>ITEM</t>
   </si>
@@ -198,9 +198,6 @@
     <t>TOTAL:</t>
   </si>
   <si>
-    <t>Need 3 panel mounts</t>
-  </si>
-  <si>
     <t>Need 27 wires</t>
   </si>
   <si>
@@ -223,6 +220,21 @@
   </si>
   <si>
     <t>Need 4 washers</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1439</t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/1440</t>
+  </si>
+  <si>
+    <t>Backlit pushbutton, Red</t>
+  </si>
+  <si>
+    <t>Backlit pushbutton, Green</t>
+  </si>
+  <si>
+    <t>Need 1 panel mount</t>
   </si>
 </sst>
 </file>
@@ -321,7 +333,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -376,6 +388,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -691,10 +704,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{299A9C15-53F9-49FA-B0A4-29D41F3B9611}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,7 +757,7 @@
         <v>5</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1201,7 +1214,7 @@
       <c r="G17" s="6"/>
       <c r="H17" s="10"/>
       <c r="I17" s="11">
-        <f t="shared" ref="I17:I26" si="2">H17*D17</f>
+        <f t="shared" ref="I17:I28" si="2">H17*D17</f>
         <v>0</v>
       </c>
       <c r="J17" s="6"/>
@@ -1216,7 +1229,7 @@
         <v>34761</v>
       </c>
       <c r="D18" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>43</v>
@@ -1232,122 +1245,128 @@
       </c>
       <c r="I18" s="11">
         <f t="shared" si="2"/>
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="J18" s="6"/>
       <c r="K18" s="6"/>
     </row>
-    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="6">
-        <v>333973</v>
+        <v>1439</v>
       </c>
       <c r="D19" s="6">
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>44</v>
+        <v>65</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>48</v>
+        <v>7</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>63</v>
       </c>
       <c r="H19" s="10">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="I19" s="11">
         <f t="shared" si="2"/>
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
     </row>
-    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="6"/>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>41</v>
+      </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6">
-        <v>23077</v>
+        <v>1440</v>
       </c>
       <c r="D20" s="6">
         <v>1</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>51</v>
+        <v>66</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>50</v>
+        <v>7</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>64</v>
       </c>
       <c r="H20" s="10">
-        <v>0.17</v>
+        <v>1.5</v>
       </c>
       <c r="I20" s="11">
         <f t="shared" si="2"/>
-        <v>0.17</v>
-      </c>
-      <c r="J20" s="6" t="s">
-        <v>55</v>
-      </c>
+        <v>1.5</v>
+      </c>
+      <c r="J20" s="6"/>
       <c r="K20" s="6"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="6">
+        <v>333973</v>
+      </c>
       <c r="D21" s="6">
         <v>1</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="10"/>
+        <v>44</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.25</v>
+      </c>
       <c r="I21" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
     </row>
-    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
-        <v>41</v>
-      </c>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="6"/>
       <c r="B22" s="6"/>
-      <c r="C22" s="16">
-        <v>2260746</v>
+      <c r="C22" s="6">
+        <v>23077</v>
       </c>
       <c r="D22" s="6">
         <v>1</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>36</v>
       </c>
       <c r="G22" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H22" s="10">
-        <v>4.95</v>
+        <v>0.17</v>
       </c>
       <c r="I22" s="11">
         <f t="shared" si="2"/>
-        <v>4.95</v>
+        <v>0.17</v>
       </c>
       <c r="J22" s="6" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="K22" s="6"/>
     </row>
@@ -1361,7 +1380,7 @@
         <v>1</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -1371,27 +1390,39 @@
         <v>0</v>
       </c>
       <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
+      <c r="C24" s="16">
+        <v>2260746</v>
+      </c>
+      <c r="D24" s="6">
+        <v>1</v>
+      </c>
       <c r="E24" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="10"/>
+        <v>47</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H24" s="10">
+        <v>4.95</v>
+      </c>
       <c r="I24" s="11">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>4.95</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>61</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="K24" s="6"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
@@ -1399,9 +1430,11 @@
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="6">
+        <v>1</v>
+      </c>
       <c r="E25" s="6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
@@ -1410,9 +1443,7 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J25" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
@@ -1422,7 +1453,7 @@
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
       <c r="E26" s="6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
@@ -1432,47 +1463,89 @@
         <v>0</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
-        <v>53</v>
+      <c r="A27" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
+      <c r="E27" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="10"/>
-      <c r="I27" s="17">
-        <f>SUM(I16:I26)</f>
-        <v>9.620000000000001</v>
-      </c>
-      <c r="J27" s="6"/>
+      <c r="I27" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="17">
+        <f>SUM(I16:I28)</f>
+        <v>12.47</v>
+      </c>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="10"/>
-      <c r="I28" s="19">
-        <f>I13+I27</f>
-        <v>86.570000000000007</v>
-      </c>
-      <c r="J28" s="4"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="6"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="19">
+        <f>I13+I29</f>
+        <v>89.42</v>
+      </c>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1487,12 +1560,14 @@
     <hyperlink ref="G5" r:id="rId9" xr:uid="{45C18FA8-746F-46E1-983D-43A1F196619C}"/>
     <hyperlink ref="G9" r:id="rId10" xr:uid="{16377B9E-2C48-417F-ADA4-C3DFFB3E9109}"/>
     <hyperlink ref="G6" r:id="rId11" xr:uid="{A9099EEE-A2B0-409A-8EBE-B199FF931F3B}"/>
-    <hyperlink ref="G19" r:id="rId12" xr:uid="{BD9211FB-2BFC-40B1-9558-856B86F0C9F4}"/>
+    <hyperlink ref="G21" r:id="rId12" xr:uid="{BD9211FB-2BFC-40B1-9558-856B86F0C9F4}"/>
     <hyperlink ref="G18" r:id="rId13" xr:uid="{B771BEF0-2490-4458-A86F-E3E407D05A91}"/>
-    <hyperlink ref="G20" r:id="rId14" xr:uid="{1ACAF4DD-20DD-4B97-BCDE-2D1427CF2FC5}"/>
-    <hyperlink ref="G22" r:id="rId15" xr:uid="{A613B684-B82A-4CD3-A9A4-C625BB4B7DDA}"/>
+    <hyperlink ref="G22" r:id="rId14" xr:uid="{1ACAF4DD-20DD-4B97-BCDE-2D1427CF2FC5}"/>
+    <hyperlink ref="G24" r:id="rId15" xr:uid="{A613B684-B82A-4CD3-A9A4-C625BB4B7DDA}"/>
+    <hyperlink ref="G19" r:id="rId16" xr:uid="{4EC62ABD-9153-40BA-A6E4-F1C367294432}"/>
+    <hyperlink ref="G20" r:id="rId17" xr:uid="{CF38DB4A-B127-40C4-A693-75C9CCBA8970}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>